<commit_message>
Andrew preliminary discharge coding
</commit_message>
<xml_diff>
--- a/Outputs/Discharge/Rating Curve Plots with Skewed Points.xlsx
+++ b/Outputs/Discharge/Rating Curve Plots with Skewed Points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nehemiah\Desktop\Ecuador\Outputs\Discharge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARMur\OneDrive - University of North Carolina at Chapel Hill\Ecuador\Github\Ecuador\Outputs\Discharge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A619554A-6B8D-48FB-ACED-E02F22611694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A619554A-6B8D-48FB-ACED-E02F22611694}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{39153BFD-3647-47FF-9D91-FA20615FCF04}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{3D4B17CD-1B51-437D-8BCB-58CF5AAF363D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3D4B17CD-1B51-437D-8BCB-58CF5AAF363D}"/>
   </bookViews>
   <sheets>
     <sheet name="Station 1 Rating Curve" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,12 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -5061,23 +5067,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A749A7-02E1-4E99-AF70-C279FF5E3264}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" customWidth="1"/>
+    <col min="3" max="4" width="11.47265625" customWidth="1"/>
+    <col min="5" max="5" width="12.47265625" customWidth="1"/>
+    <col min="6" max="6" width="9.15625" customWidth="1"/>
+    <col min="7" max="7" width="14.26171875" customWidth="1"/>
+    <col min="8" max="8" width="12.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -5103,7 +5106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5117,7 +5120,7 @@
         <v>3.925E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5134,7 +5137,7 @@
         <v>1.7146927999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -5151,7 +5154,7 @@
         <v>0.16889999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -5160,7 +5163,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -5177,7 +5180,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -5208,7 +5211,7 @@
         <v>0.17609520000000067</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -5239,7 +5242,7 @@
         <v>0.19591900000000084</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -5270,7 +5273,7 @@
         <v>-4.0472999999998649E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -5278,7 +5281,7 @@
         <v>43672</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -5295,7 +5298,7 @@
         <v>0.16220000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -5312,7 +5315,7 @@
         <v>0.15490000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -5329,7 +5332,10 @@
         <v>0.15490000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
       <c r="B14" s="1">
         <v>43684</v>
       </c>
@@ -5350,16 +5356,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E78F823-04A9-482A-86C2-E79FA16E1913}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="5" max="5" width="10.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.3671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -5376,7 +5382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -5390,7 +5396,7 @@
         <v>1.0425E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5404,7 +5410,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -5421,7 +5427,7 @@
         <v>0.1699</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -5438,7 +5444,7 @@
         <v>0.43280000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -5455,7 +5461,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -5472,7 +5478,7 @@
         <v>0.16969999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5489,7 +5495,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -5506,7 +5512,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -5523,7 +5529,7 @@
         <v>0.21529999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5534,7 +5540,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -5551,7 +5557,7 @@
         <v>0.1454</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5568,7 +5574,7 @@
         <v>0.19189999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -5594,16 +5600,16 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10.89453125" customWidth="1"/>
+    <col min="5" max="5" width="11.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -5620,7 +5626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5631,7 +5637,7 @@
         <v>4.4850000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -5642,7 +5648,7 @@
         <v>3.9274999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -5651,7 +5657,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -5662,7 +5668,7 @@
         <v>6.5449999999999994E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5673,7 +5679,7 @@
         <v>5.1075000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -5690,7 +5696,7 @@
         <v>0.2102458696</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -5707,7 +5713,7 @@
         <v>0.24191327419999997</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -5724,7 +5730,7 @@
         <v>0.32168087119999994</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -5741,7 +5747,7 @@
         <v>0.2443555036</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -5758,7 +5764,7 @@
         <v>0.17703358919999998</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -5775,7 +5781,7 @@
         <v>0.1606059</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5792,7 +5798,7 @@
         <v>0.19554150719999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -5817,16 +5823,16 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="E2" sqref="E2:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="10.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5234375" customWidth="1"/>
+    <col min="5" max="5" width="11.7890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -5843,7 +5849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5854,7 +5860,7 @@
         <v>2.01E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5865,7 +5871,7 @@
         <v>2.7404999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -5876,7 +5882,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -5887,7 +5893,7 @@
         <v>0.1087</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -5898,7 +5904,7 @@
         <v>5.0549999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5915,7 +5921,7 @@
         <v>0.21569627299999997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -5932,7 +5938,7 @@
         <v>0.24453905319999997</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -5949,7 +5955,7 @@
         <v>0.31944768439999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -5966,7 +5972,7 @@
         <v>0.24490615239999997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -5983,7 +5989,7 @@
         <v>0.17671747599999998</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -6000,7 +6006,7 @@
         <v>0.16108516840000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -6017,7 +6023,7 @@
         <v>0.19817238479999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Level logger data cleaning, still need 2020425 and 2020432. Everything else adjusted
</commit_message>
<xml_diff>
--- a/Outputs/Discharge/Rating Curve Plots with Skewed Points.xlsx
+++ b/Outputs/Discharge/Rating Curve Plots with Skewed Points.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARMur\OneDrive - University of North Carolina at Chapel Hill\Ecuador\Github\Ecuador\Outputs\Discharge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/armurray_ad_unc_edu/Documents/Ecuador/Github/Ecuador/Outputs/Discharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A619554A-6B8D-48FB-ACED-E02F22611694}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{39153BFD-3647-47FF-9D91-FA20615FCF04}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{A619554A-6B8D-48FB-ACED-E02F22611694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{05F2770C-A33D-49D3-9A83-3E2494860B60}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3D4B17CD-1B51-437D-8BCB-58CF5AAF363D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{3D4B17CD-1B51-437D-8BCB-58CF5AAF363D}"/>
   </bookViews>
   <sheets>
     <sheet name="Station 1 Rating Curve" sheetId="1" r:id="rId1"/>
-    <sheet name="Station 2 Rating Curve" sheetId="2" r:id="rId2"/>
-    <sheet name="Station 3 Rating Curve" sheetId="3" r:id="rId3"/>
-    <sheet name="Station 4 Rating Curve" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Station 2 Rating Curve" sheetId="2" r:id="rId3"/>
+    <sheet name="Station 3 Rating Curve" sheetId="3" r:id="rId4"/>
+    <sheet name="Station 4 Rating Curve" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="21">
   <si>
     <t>Station 1</t>
   </si>
@@ -5067,8 +5069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A749A7-02E1-4E99-AF70-C279FF5E3264}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5353,11 +5355,700 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3AC49B-32F5-41A4-A1C1-1B8F971BF409}">
+  <dimension ref="A1:D48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="8.3671875" customWidth="1"/>
+    <col min="3" max="3" width="14.83984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43656</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="D2">
+        <v>3.925E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43657</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D3">
+        <v>6.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43658</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D4">
+        <v>9.1199999999999996E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43662</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D5">
+        <v>1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43665</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D6">
+        <v>1.4345E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43668</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D7">
+        <v>2.0525000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43670</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D8">
+        <v>6.0824999999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43678</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D9">
+        <v>6.0499999999999998E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43679</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="D10">
+        <v>5.874999999999928E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43682</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="D11">
+        <v>1.1462500000000205E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43684</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.4465277777777778</v>
+      </c>
+      <c r="D12">
+        <v>1.9750000000000119E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43656</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>1.0425E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43657</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D14">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>43658</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D15">
+        <v>9.1199999999999996E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43661</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3.5099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>43662</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D17">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43665</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="D18">
+        <v>8.1799999999999998E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43668</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="D19">
+        <v>1.788E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43670</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D20">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43672</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D21">
+        <v>1.6899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43679</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="D22">
+        <v>4.5500000000000002E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43682</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D23">
+        <v>1.3480000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1">
+        <v>43684</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D24">
+        <v>6.4700000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <v>43656</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D25">
+        <v>4.4850000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1">
+        <v>43657</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D26">
+        <v>3.9274999999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1">
+        <v>43661</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D27">
+        <v>6.5449999999999994E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>43662</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D28">
+        <v>5.1075000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1">
+        <v>43665</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D29">
+        <v>2.41E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1">
+        <v>43668</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D30">
+        <v>4.6199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="1">
+        <v>43670</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="D31">
+        <v>0.14369999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1">
+        <v>43672</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D32">
+        <v>6.0475000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1">
+        <v>43678</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D33">
+        <v>1.3950000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1">
+        <v>43679</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D34">
+        <v>1.8575000000000015E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1">
+        <v>43682</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D35">
+        <v>3.7525000000000093E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <v>43684</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D36">
+        <v>1.6750000000000022E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1">
+        <v>43656</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D37">
+        <v>2.01E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1">
+        <v>43657</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D38">
+        <v>2.7404999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1">
+        <v>43661</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D39">
+        <v>0.1087</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1">
+        <v>43662</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D40">
+        <v>5.0549999999999998E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1">
+        <v>43665</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D41">
+        <v>1.0187999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1">
+        <v>43668</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D42">
+        <v>2.6025E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="1">
+        <v>43670</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D43">
+        <v>9.9900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1">
+        <v>43672</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="D44">
+        <v>2.8049999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1">
+        <v>43678</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D45">
+        <v>7.6499999999999997E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1">
+        <v>43679</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D46">
+        <v>7.0750000000000847E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1">
+        <v>43682</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D47">
+        <v>1.9800000000000109E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1">
+        <v>43684</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="D48">
+        <v>6.8250000000000142E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E78F823-04A9-482A-86C2-E79FA16E1913}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="A2" sqref="A2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5595,12 +6286,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8C54F8-6061-4B44-A50B-FAFFEB9E577C}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A2" sqref="A2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5818,12 +6509,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFD2133-FBE0-4AE7-B42A-9E594457259C}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E14"/>
+      <selection activeCell="A2" sqref="A2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
data merge update with EC and DO
</commit_message>
<xml_diff>
--- a/Outputs/Discharge/Rating Curve Plots with Skewed Points.xlsx
+++ b/Outputs/Discharge/Rating Curve Plots with Skewed Points.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/armurray_ad_unc_edu/Documents/Ecuador/Github/Ecuador/Outputs/Discharge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARMur\OneDrive - University of North Carolina at Chapel Hill\Ecuador\Github\Ecuador\Outputs\Discharge\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{A619554A-6B8D-48FB-ACED-E02F22611694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{05F2770C-A33D-49D3-9A83-3E2494860B60}"/>
@@ -20,7 +20,6 @@
     <sheet name="Station 4 Rating Curve" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5358,8 +5357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3AC49B-32F5-41A4-A1C1-1B8F971BF409}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>